<commit_message>
UTS - Perbaikan error/bug
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS_2024\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17616068-84E6-46D9-A44F-F1BDF3DE47B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE07813-7058-4253-8641-8DD5C7C4A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{23C09CB0-45CD-4FF6-B511-2FBD0E6B9263}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="9420" xr2:uid="{23C09CB0-45CD-4FF6-B511-2FBD0E6B9263}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>kategori_id</t>
   </si>
@@ -51,34 +51,10 @@
     <t>harga_jual</t>
   </si>
   <si>
-    <t>SBK-003</t>
-  </si>
-  <si>
-    <t>Telur omega(10 butir)</t>
-  </si>
-  <si>
-    <t>SNK-003</t>
-  </si>
-  <si>
-    <t>Selai Roti</t>
-  </si>
-  <si>
-    <t>MND-003</t>
-  </si>
-  <si>
-    <t>Shampo Pantene</t>
-  </si>
-  <si>
-    <t>BAY-003</t>
-  </si>
-  <si>
-    <t>Baju Bayi 2th</t>
-  </si>
-  <si>
-    <t>MNM-003</t>
-  </si>
-  <si>
-    <t>Cleo 600ml</t>
+    <t>SBW</t>
+  </si>
+  <si>
+    <t>Sabun Wajah</t>
   </si>
 </sst>
 </file>
@@ -127,10 +103,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,7 +426,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,79 +464,39 @@
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>22000</v>
+        <v>22300</v>
       </c>
       <c r="E2" s="2">
-        <v>25000</v>
+        <v>25300</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>11500</v>
-      </c>
-      <c r="E3" s="2">
-        <v>12500</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>17500</v>
-      </c>
-      <c r="E4" s="2">
-        <v>18500</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2">
-        <v>89000</v>
-      </c>
-      <c r="E5" s="2">
-        <v>92500</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3750</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4300</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>